<commit_message>
Remove data cruft so group file can be processed by etl scripts
</commit_message>
<xml_diff>
--- a/data/GroupingsOBSQuestions2017.xlsx
+++ b/data/GroupingsOBSQuestions2017.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Y_Open Knowledge Data\for open knowledge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brew/Documents/Work/OpenKnowledge/ibp/ibp-explorer/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26420" windowHeight="19600" tabRatio="992"/>
   </bookViews>
   <sheets>
     <sheet name="QuestionsGroups 2015" sheetId="1" r:id="rId1"/>
@@ -17,11 +17,19 @@
     <sheet name="CountriesRegions 2015-17" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="174">
   <si>
     <t>Groupings for the OBS Questions (based on the 2015 Questionnaire)</t>
   </si>
@@ -521,9 +529,6 @@
     <t>97-102,t3ar</t>
   </si>
   <si>
-    <t>1-102, t3pbs, t3ebp, t3eb, t3iyr, t3myr, t3yer, t3ar</t>
-  </si>
-  <si>
     <t>125-142</t>
   </si>
   <si>
@@ -542,58 +547,10 @@
     <t>119-124</t>
   </si>
   <si>
-    <t>Note: if possible, we would like to show the following question numbers in 2015 and 2017, respectively</t>
-  </si>
-  <si>
-    <t>2015 value</t>
-  </si>
-  <si>
-    <t>2017 value</t>
-  </si>
-  <si>
-    <t>t3pbs</t>
-  </si>
-  <si>
-    <t>t3ebp</t>
-  </si>
-  <si>
-    <t>t3eb</t>
-  </si>
-  <si>
-    <t>t3iyr</t>
-  </si>
-  <si>
-    <t>t3myr</t>
-  </si>
-  <si>
-    <t>t3yer</t>
-  </si>
-  <si>
-    <t>t3ar</t>
-  </si>
-  <si>
-    <t>PBS-2</t>
-  </si>
-  <si>
-    <t>EBP-2</t>
-  </si>
-  <si>
-    <t>EB-2</t>
-  </si>
-  <si>
-    <t>IYR-2</t>
-  </si>
-  <si>
-    <t>MYR-2</t>
-  </si>
-  <si>
-    <t>YER-2</t>
-  </si>
-  <si>
-    <t>AR-2</t>
-  </si>
-  <si>
     <t>Groupings for the OBS Questions (based on the 2017 Questionnaire)</t>
+  </si>
+  <si>
+    <t>1-102, 143-149</t>
   </si>
 </sst>
 </file>
@@ -826,9 +783,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -861,9 +818,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1043,24 +1000,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="1025" width="8.85546875"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="41.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1068,16 +1024,16 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3"/>
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1088,7 +1044,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1099,7 +1055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1110,10 +1066,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="B8" s="4" t="s">
         <v>8</v>
@@ -1122,7 +1078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1133,7 +1089,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -1144,7 +1100,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -1155,7 +1111,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -1166,7 +1122,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>5</v>
       </c>
@@ -1177,7 +1133,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>6</v>
       </c>
@@ -1188,7 +1144,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>7</v>
       </c>
@@ -1199,7 +1155,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -1210,16 +1166,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -1230,7 +1186,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -1241,7 +1197,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>3</v>
       </c>
@@ -1252,7 +1208,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>4</v>
       </c>
@@ -1273,29 +1229,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="41.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1303,10 +1259,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1314,10 +1270,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1325,35 +1281,35 @@
         <v>6</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3.1</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>3.2</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -1361,7 +1317,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1372,7 +1328,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -1383,7 +1339,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -1394,7 +1350,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>4</v>
       </c>
@@ -1405,7 +1361,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>5</v>
       </c>
@@ -1416,7 +1372,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>6</v>
       </c>
@@ -1427,7 +1383,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>7</v>
       </c>
@@ -1438,7 +1394,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>8</v>
       </c>
@@ -1449,12 +1405,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -1465,7 +1421,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -1476,7 +1432,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>3</v>
       </c>
@@ -1487,7 +1443,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>4</v>
       </c>
@@ -1498,74 +1454,33 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>176</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>177</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>178</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>179</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>180</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>181</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>182</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>189</v>
-      </c>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="11"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="12"/>
+      <c r="B29" s="13"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="11"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B31" s="11"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B32" s="11"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="11"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="11"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" s="11"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1575,26 +1490,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:AMI38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="19.5703125" style="5"/>
-    <col min="4" max="4" width="24.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="19.5" style="5"/>
+    <col min="4" max="4" width="24.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="19.5703125" style="5"/>
-    <col min="8" max="8" width="33.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="1023" width="19.5703125" style="5"/>
+    <col min="6" max="7" width="19.5" style="5"/>
+    <col min="8" max="8" width="33.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="1023" width="19.5" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
@@ -1606,7 +1521,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -1616,7 +1531,7 @@
       <c r="G2"/>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>36</v>
       </c>
@@ -1642,7 +1557,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>147</v>
       </c>
@@ -1668,7 +1583,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
@@ -1694,7 +1609,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>51</v>
       </c>
@@ -1720,7 +1635,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>59</v>
       </c>
@@ -1746,7 +1661,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>67</v>
       </c>
@@ -1772,7 +1687,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>150</v>
       </c>
@@ -1798,7 +1713,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>75</v>
       </c>
@@ -1818,7 +1733,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>83</v>
       </c>
@@ -1838,7 +1753,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>91</v>
       </c>
@@ -1858,7 +1773,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>97</v>
       </c>
@@ -1878,7 +1793,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>103</v>
       </c>
@@ -1892,7 +1807,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>109</v>
       </c>
@@ -1906,7 +1821,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>114</v>
       </c>
@@ -1920,7 +1835,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>118</v>
       </c>
@@ -1934,7 +1849,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>122</v>
       </c>
@@ -1948,7 +1863,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>126</v>
       </c>
@@ -1959,7 +1874,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D20" s="5" t="s">
         <v>132</v>
       </c>
@@ -1967,92 +1882,92 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G21" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G22" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G23" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G24" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G25" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G26" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G27" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G28" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G29" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G30" s="10" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G31" s="5" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G32" s="10" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G33" s="5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G34" s="10" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G35" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G36" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G37" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G38" s="5" t="s">
         <v>144</v>
       </c>

</xml_diff>

<commit_message>
Fix Groupings for 2017
- Change oversights label
- Change t3* question labels to numbers so they work in the report
generator
</commit_message>
<xml_diff>
--- a/data/GroupingsOBSQuestions2017.xlsx
+++ b/data/GroupingsOBSQuestions2017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26420" windowHeight="19600" tabRatio="992"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26420" windowHeight="19600" tabRatio="992" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="QuestionsGroups 2015" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="175">
   <si>
     <t>Groupings for the OBS Questions (based on the 2015 Questionnaire)</t>
   </si>
@@ -508,27 +508,6 @@
     <t>Western Europe, U.S. &amp; Canada</t>
   </si>
   <si>
-    <t>54-58, t3pbs</t>
-  </si>
-  <si>
-    <t>1-53, t3ebp</t>
-  </si>
-  <si>
-    <t>59-63, t3eb</t>
-  </si>
-  <si>
-    <t>68-75, t3iyr</t>
-  </si>
-  <si>
-    <t>76-83, t3myr</t>
-  </si>
-  <si>
-    <t>84-96, t3yer</t>
-  </si>
-  <si>
-    <t>97-102,t3ar</t>
-  </si>
-  <si>
     <t>125-142</t>
   </si>
   <si>
@@ -551,6 +530,30 @@
   </si>
   <si>
     <t>1-102, 143-149</t>
+  </si>
+  <si>
+    <t>Role and Effectiveness of Oversight Institutions</t>
+  </si>
+  <si>
+    <t>1-53, 144</t>
+  </si>
+  <si>
+    <t>59-63, 145</t>
+  </si>
+  <si>
+    <t>68-75, 146</t>
+  </si>
+  <si>
+    <t>76-83, 147</t>
+  </si>
+  <si>
+    <t>84-96, 148</t>
+  </si>
+  <si>
+    <t>97-102, 149</t>
+  </si>
+  <si>
+    <t>54-58, 143</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1008,7 @@
   </sheetPr>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1229,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1241,7 +1244,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="2"/>
@@ -1259,7 +1262,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1270,7 +1273,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1278,10 +1281,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>6</v>
+        <v>167</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1289,10 +1292,10 @@
         <v>3.1</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1300,10 +1303,10 @@
         <v>3.2</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1325,7 +1328,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1336,7 +1339,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1347,7 +1350,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1369,7 +1372,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1380,7 +1383,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1391,7 +1394,7 @@
         <v>22</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1402,7 +1405,7 @@
         <v>24</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>